<commit_message>
se agrega indicadores financieros
</commit_message>
<xml_diff>
--- a/Analisis financiero Inclusoft.xlsx
+++ b/Analisis financiero Inclusoft.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" tabRatio="920" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" tabRatio="920" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Presupuesto Inicial" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="281">
   <si>
     <t xml:space="preserve">Concepto
 </t>
@@ -903,26 +903,33 @@
     <t>VPN 1+</t>
   </si>
   <si>
-    <t>Tasa de interes minima aceptable</t>
+    <t>VPN con Tasa de interes</t>
+  </si>
+  <si>
+    <t>Tasa de interes de oportunidad</t>
+  </si>
+  <si>
+    <t>vpn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="[$$-240A]\ #,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$$-240A]\ #,##0"/>
     <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="178" formatCode="0.0000"/>
-    <numFmt numFmtId="180" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="181" formatCode="_-[$$-240A]\ * #,##0.000_-;\-[$$-240A]\ * #,##0.000_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="183" formatCode="_-[$$-240A]\ * #,##0.000_-;\-[$$-240A]\ * #,##0.000_-;_-[$$-240A]\ * &quot;-&quot;???_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="171" formatCode="_-[$$-240A]\ * #,##0.000_-;\-[$$-240A]\ * #,##0.000_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="172" formatCode="_-[$$-240A]\ * #,##0.000_-;\-[$$-240A]\ * #,##0.000_-;_-[$$-240A]\ * &quot;-&quot;???_-;_-@_-"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1058,8 +1065,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1080,6 +1092,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
   </fills>
@@ -1307,14 +1325,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="213">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1583,16 +1602,83 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="11" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="18" fillId="3" borderId="11" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="2"/>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="19" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1601,31 +1687,6 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="12" xfId="3"/>
     <xf numFmtId="164" fontId="19" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1664,57 +1725,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="18" fillId="3" borderId="11" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="18" fillId="3" borderId="11" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="2"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="2"/>
-    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="17" xfId="2" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="25" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Celda de comprobación" xfId="3" builtinId="23"/>
+    <cellStyle name="Millares" xfId="5" builtinId="3"/>
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="4" builtinId="5"/>
@@ -1859,46 +1892,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="[$$-240A]\ #,##0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="178" formatCode="0.0000"/>
+      <numFmt numFmtId="169" formatCode="0.0000"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1939,6 +1933,9 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="167" formatCode="[$$-240A]\ #,##0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1954,7 +1951,61 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="180" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="170" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2027,24 +2078,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -2053,6 +2086,20 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -2079,6 +2126,23 @@
       </font>
       <numFmt numFmtId="167" formatCode="[$$-240A]\ #,##0"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="[$$-240A]\ #,##0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2127,86 +2191,8 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="167" formatCode="[$$-240A]\ #,##0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2259,21 +2245,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="[$$-240A]\ #,##0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -2286,24 +2257,22 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="[$$-240A]\ #,##0"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2342,6 +2311,38 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2361,6 +2362,38 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2483,7 +2516,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2641,8 +2673,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="408626952"/>
-        <c:axId val="408628520"/>
+        <c:axId val="259893648"/>
+        <c:axId val="301302136"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -2730,7 +2762,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="408626952"/>
+        <c:axId val="259893648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2762,7 +2794,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2829,7 +2860,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="408628520"/>
+        <c:crossAx val="301302136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2837,7 +2868,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="408628520"/>
+        <c:axId val="301302136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2951,7 +2982,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="408626952"/>
+        <c:crossAx val="259893648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2975,7 +3006,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3094,10 +3124,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'VAN y TIR'!$L$6:$L$43</c:f>
+              <c:f>'VAN y TIR'!$L$6:$L$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3164,13 +3194,13 @@
                 <c:pt idx="21">
                   <c:v>1.05</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>1.1000000000000001</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>1.1499999999999999</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="39">
                   <c:v>1.2</c:v>
                 </c:pt>
               </c:numCache>
@@ -3178,10 +3208,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'VAN y TIR'!$M$6:$M$43</c:f>
+              <c:f>'VAN y TIR'!$M$6:$M$45</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00</c:formatCode>
-                <c:ptCount val="38"/>
+                <c:ptCount val="40"/>
                 <c:pt idx="0">
                   <c:v>8928555557.1527557</c:v>
                 </c:pt>
@@ -3248,13 +3278,13 @@
                 <c:pt idx="21">
                   <c:v>913716919.97802794</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="37">
                   <c:v>855330893.90745759</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="38">
                   <c:v>802348473.35562515</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="39">
                   <c:v>754126147.23541009</c:v>
                 </c:pt>
               </c:numCache>
@@ -3271,11 +3301,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="307580176"/>
-        <c:axId val="308033632"/>
+        <c:axId val="301302528"/>
+        <c:axId val="301302920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="307580176"/>
+        <c:axId val="301302528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3318,7 +3348,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="308033632"/>
+        <c:crossAx val="301302920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3326,7 +3356,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="308033632"/>
+        <c:axId val="301302920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3383,7 +3413,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="307580176"/>
+        <c:crossAx val="301302528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4255,26 +4285,26 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="PUBLICIDAD" displayName="PUBLICIDAD" ref="A36:H43" totalsRowCount="1" headerRowDxfId="40" totalsRowDxfId="39" headerRowCellStyle="Celda de comprobación">
   <tableColumns count="8">
     <tableColumn id="1" name="Promoción" dataDxfId="38"/>
-    <tableColumn id="2" name="Tiempo aproximado de duración" dataDxfId="37" totalsRowDxfId="30"/>
-    <tableColumn id="3" name="Objetivo " dataDxfId="36" totalsRowDxfId="29"/>
-    <tableColumn id="4" name="Cantidad" dataDxfId="35" totalsRowDxfId="28"/>
-    <tableColumn id="5" name="Se requieren" dataDxfId="34" totalsRowDxfId="27"/>
-    <tableColumn id="6" name="Costo Unitario" totalsRowLabel="Total" dataDxfId="33" totalsRowDxfId="26" dataCellStyle="Moneda"/>
-    <tableColumn id="7" name="Costo total" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="25" dataCellStyle="Moneda">
+    <tableColumn id="2" name="Tiempo aproximado de duración" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" name="Objetivo " dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="4" name="Cantidad" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="5" name="Se requieren" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="6" name="Costo Unitario" totalsRowLabel="Total" dataDxfId="29" totalsRowDxfId="28" dataCellStyle="Moneda"/>
+    <tableColumn id="7" name="Costo total" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26" dataCellStyle="Moneda">
       <calculatedColumnFormula>F37*E37</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Proveedor" dataDxfId="31" totalsRowDxfId="24"/>
+    <tableColumn id="8" name="Proveedor" dataDxfId="25" totalsRowDxfId="24"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A21:G23" totalsRowShown="0" headerRowDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabla3" displayName="Tabla3" ref="A21:G23" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="A21:G23"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Columna1"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="23"/>
+    <tableColumn id="2" name="Columna2" dataDxfId="22"/>
     <tableColumn id="3" name="Columna3">
       <calculatedColumnFormula>'Flujo de Caja (Profesor) - 5 añ'!D18</calculatedColumnFormula>
     </tableColumn>
@@ -4296,12 +4326,12 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="A30:B32" totalsRowShown="0">
-  <autoFilter ref="A30:B32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabla5" displayName="Tabla5" ref="A31:B34" totalsRowShown="0">
+  <autoFilter ref="A31:B34"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Columna1" dataDxfId="21"/>
     <tableColumn id="2" name="Columna2">
-      <calculatedColumnFormula>B30*2</calculatedColumnFormula>
+      <calculatedColumnFormula>B31*2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4309,8 +4339,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="A34:B39" totalsRowShown="0">
-  <autoFilter ref="A34:B39"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabla6" displayName="Tabla6" ref="A36:B41" totalsRowShown="0">
+  <autoFilter ref="A36:B41"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Columna1" dataDxfId="20"/>
     <tableColumn id="2" name="Columna2" dataDxfId="19"/>
@@ -4320,25 +4350,25 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="A25:C27" totalsRowShown="0">
-  <autoFilter ref="A25:C27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla4" displayName="Tabla4" ref="A25:C28" totalsRowShown="0">
+  <autoFilter ref="A25:C28"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Columna1" dataDxfId="14"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="13"/>
-    <tableColumn id="3" name="Columna3" dataDxfId="15"/>
+    <tableColumn id="1" name="Columna1" dataDxfId="18"/>
+    <tableColumn id="2" name="Columna2" dataDxfId="17"/>
+    <tableColumn id="3" name="Columna3" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A43:C49" totalsRowShown="0">
-  <autoFilter ref="A43:C49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A45:C51" totalsRowShown="0">
+  <autoFilter ref="A45:C51"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Columna1" dataDxfId="18"/>
-    <tableColumn id="2" name="Columna2" dataDxfId="17" dataCellStyle="Porcentaje"/>
-    <tableColumn id="3" name="Columna3" dataDxfId="16" dataCellStyle="Porcentaje">
-      <calculatedColumnFormula xml:space="preserve"> 1 +B44</calculatedColumnFormula>
+    <tableColumn id="1" name="Columna1" dataDxfId="15"/>
+    <tableColumn id="2" name="Columna2" dataDxfId="14" dataCellStyle="Porcentaje"/>
+    <tableColumn id="3" name="Columna3" dataDxfId="13" dataCellStyle="Porcentaje">
+      <calculatedColumnFormula xml:space="preserve"> 1 +B46</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4941,9 +4971,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -4978,7 +5008,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
       <c r="A2" s="100" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B2" s="11">
         <v>0.15</v>
@@ -5090,7 +5120,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="44">
-        <f t="shared" ref="M6:M43" si="0">NPV(L6,$J$2:$J$6)+$J$1</f>
+        <f t="shared" ref="M6:M45" si="0">NPV(L6,$J$2:$J$6)+$J$1</f>
         <v>8928555557.1527557</v>
       </c>
     </row>
@@ -5318,7 +5348,9 @@
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1">
       <c r="A22" s="120"/>
-      <c r="B22" s="120"/>
+      <c r="B22" s="150" t="s">
+        <v>77</v>
+      </c>
       <c r="C22" s="98" t="s">
         <v>74</v>
       </c>
@@ -5346,24 +5378,27 @@
       <c r="A23" s="119" t="s">
         <v>261</v>
       </c>
-      <c r="B23" s="120"/>
-      <c r="C23" s="206">
+      <c r="B23" s="217">
+        <f>B1*-1</f>
+        <v>-62189202</v>
+      </c>
+      <c r="C23" s="171">
         <f>'Flujo de Caja (Profesor) - 5 añ'!D19</f>
         <v>413409873.08069575</v>
       </c>
-      <c r="D23" s="206">
+      <c r="D23" s="171">
         <f>'Flujo de Caja (Profesor) - 5 añ'!F19</f>
         <v>1215891380.9377983</v>
       </c>
-      <c r="E23" s="206">
+      <c r="E23" s="171">
         <f>'Flujo de Caja (Profesor) - 5 añ'!H19</f>
         <v>2365721712.3720331</v>
       </c>
-      <c r="F23" s="206">
+      <c r="F23" s="171">
         <f>'Flujo de Caja (Profesor) - 5 añ'!J19</f>
         <v>2494107299.486268</v>
       </c>
-      <c r="G23" s="206">
+      <c r="G23" s="171">
         <f>'Flujo de Caja (Profesor) - 5 añ'!L19</f>
         <v>2501615291.2759619</v>
       </c>
@@ -5392,7 +5427,7 @@
       <c r="B25" s="120" t="s">
         <v>266</v>
       </c>
-      <c r="C25" s="207" t="s">
+      <c r="C25" s="172" t="s">
         <v>267</v>
       </c>
       <c r="L25" s="11">
@@ -5408,8 +5443,8 @@
         <v>262</v>
       </c>
       <c r="B26" s="120"/>
-      <c r="C26" s="207">
-        <f>J1+(C23/C45)+(D23/C45*C46)+(E23/C45*C46*C47)+(F23/C45*C46*C47*C48)+(G23/C45*C46*C47*C48*C49)</f>
+      <c r="C26" s="172">
+        <f>J1+(C23/C47)+(D23/C47*C48)+(E23/C47*C48*C49)+(F23/C47*C48*C49*C50)+(G23/C47*C48*C49*C50*C51)</f>
         <v>9985027796.3041878</v>
       </c>
       <c r="L26" s="11">
@@ -5421,10 +5456,14 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="12.75">
-      <c r="A27" s="119" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" s="120"/>
+      <c r="A27" s="151" t="s">
+        <v>278</v>
+      </c>
+      <c r="B27" s="151"/>
+      <c r="C27" s="172">
+        <f>-B1+(C23/(1+B2))+(D23/(1+B2)^2)+(E23/(1+B2)^3)+(F23/(1+B2)^4)+(G23/(1+B2)^5)</f>
+        <v>5441945506.1028109</v>
+      </c>
       <c r="L27" s="11">
         <v>1.05</v>
       </c>
@@ -5434,8 +5473,14 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="12.75">
-      <c r="A28" s="119"/>
-      <c r="B28" s="120"/>
+      <c r="A28" s="151" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" s="151"/>
+      <c r="C28" s="216">
+        <f>B32+((B34-B32)*(E32/(E32+E34)))</f>
+        <v>28.757062254909471</v>
+      </c>
       <c r="L28" s="11"/>
       <c r="M28" s="44"/>
     </row>
@@ -5446,230 +5491,262 @@
       <c r="M29" s="44"/>
     </row>
     <row r="30" spans="1:13" ht="12.75">
-      <c r="A30" s="119" t="s">
-        <v>265</v>
-      </c>
-      <c r="B30" s="211" t="s">
-        <v>266</v>
-      </c>
+      <c r="A30" s="119"/>
+      <c r="B30" s="120"/>
       <c r="L30" s="11"/>
       <c r="M30" s="44"/>
     </row>
     <row r="31" spans="1:13" ht="12.75">
       <c r="A31" s="119" t="s">
+        <v>265</v>
+      </c>
+      <c r="B31" s="176" t="s">
+        <v>266</v>
+      </c>
+      <c r="L31" s="11"/>
+      <c r="M31" s="44"/>
+    </row>
+    <row r="32" spans="1:13" ht="12.75">
+      <c r="A32" s="119" t="s">
         <v>272</v>
       </c>
-      <c r="B31" s="211">
+      <c r="B32" s="176">
         <f>(((C23+D23+E23+F23+G23)/B1)-1)/5</f>
         <v>28.71416923842424</v>
       </c>
-      <c r="L31" s="11"/>
-      <c r="M31" s="44"/>
-    </row>
-    <row r="32" spans="1:13" ht="12.75">
-      <c r="A32" s="119" t="s">
-        <v>273</v>
-      </c>
-      <c r="B32" s="212">
-        <f>B31*2</f>
-        <v>57.428338476848481</v>
+      <c r="D32" t="s">
+        <v>280</v>
+      </c>
+      <c r="E32" s="215">
+        <f>-$B$1+($C$23/(1+B32))+($D$23/((1+B32)^2))+($E$23/((1+B32)^3))+($F$23/((1+B32)^4))+($G$23/((1+B32)^5))</f>
+        <v>-46805728.903633773</v>
       </c>
       <c r="L32" s="11"/>
       <c r="M32" s="44"/>
     </row>
     <row r="33" spans="1:13" ht="12.75">
-      <c r="A33" s="119"/>
-      <c r="B33" s="120"/>
+      <c r="A33" s="151"/>
+      <c r="B33" s="176">
+        <v>29</v>
+      </c>
+      <c r="D33" t="s">
+        <v>280</v>
+      </c>
+      <c r="E33" s="215">
+        <f t="shared" ref="E33:E34" si="1">-$B$1+($C$23/(1+B33))+($D$23/((1+B33)^2))+($E$23/((1+B33)^3))+($F$23/((1+B33)^4))+($G$23/((1+B33)^5))</f>
+        <v>-46967081.059419967</v>
+      </c>
       <c r="L33" s="11"/>
       <c r="M33" s="44"/>
     </row>
     <row r="34" spans="1:13" ht="12.75">
       <c r="A34" s="119" t="s">
-        <v>265</v>
-      </c>
-      <c r="B34" s="210" t="s">
-        <v>266</v>
+        <v>273</v>
+      </c>
+      <c r="B34" s="177">
+        <v>28.8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>280</v>
+      </c>
+      <c r="E34" s="215">
+        <f t="shared" si="1"/>
+        <v>-46854537.664252765</v>
       </c>
       <c r="L34" s="11"/>
       <c r="M34" s="44"/>
     </row>
     <row r="35" spans="1:13" ht="12.75">
-      <c r="A35" s="119" t="s">
-        <v>274</v>
-      </c>
-      <c r="B35" s="210">
-        <f>-B1+(C23/(1+B31))+(D23/((1+B31)^2))+(E23/((1+B31)^3))+(F23/((1+B31)^4))+(G23/((1+B31)^5))</f>
-        <v>-46805728.903633773</v>
-      </c>
+      <c r="A35" s="119"/>
+      <c r="B35" s="120"/>
       <c r="L35" s="11"/>
       <c r="M35" s="44"/>
     </row>
     <row r="36" spans="1:13" ht="12.75">
       <c r="A36" s="119" t="s">
-        <v>275</v>
-      </c>
-      <c r="B36" s="210">
-        <f>-B1+(C23/(1+B32))+(D23/((1+B32)^2))+(E23/((1+B32)^3))+(F23/((1+B32)^4))+(G23/((1+B32)^5))</f>
-        <v>-54745459.181504875</v>
+        <v>265</v>
+      </c>
+      <c r="B36" s="175" t="s">
+        <v>266</v>
       </c>
       <c r="L36" s="11"/>
       <c r="M36" s="44"/>
     </row>
     <row r="37" spans="1:13" ht="12.75">
       <c r="A37" s="119" t="s">
-        <v>277</v>
-      </c>
-      <c r="B37" s="210">
-        <f>B35*-1</f>
-        <v>46805728.903633773</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="B37" s="175"/>
       <c r="L37" s="11"/>
       <c r="M37" s="44"/>
     </row>
     <row r="38" spans="1:13" ht="12.75">
       <c r="A38" s="119" t="s">
-        <v>276</v>
-      </c>
-      <c r="B38" s="210">
-        <f>B36*-1</f>
-        <v>54745459.181504875</v>
+        <v>275</v>
+      </c>
+      <c r="B38" s="175">
+        <f>-B1+(C23/(1+B34))+(D23/((1+B34)^2))+(E23/((1+B34)^3))+(F23/((1+B34)^4))+(G23/((1+B34)^5))</f>
+        <v>-46854537.664252765</v>
       </c>
       <c r="L38" s="11"/>
       <c r="M38" s="44"/>
     </row>
     <row r="39" spans="1:13" ht="12.75">
       <c r="A39" s="119" t="s">
-        <v>118</v>
-      </c>
-      <c r="B39" s="210">
-        <f>B31+(B37/(B37+B38))</f>
-        <v>29.175076981467019</v>
+        <v>277</v>
+      </c>
+      <c r="B39" s="175">
+        <f>E32*-1</f>
+        <v>46805728.903633773</v>
       </c>
       <c r="L39" s="11"/>
       <c r="M39" s="44"/>
     </row>
     <row r="40" spans="1:13" ht="12.75">
-      <c r="A40" s="119"/>
-      <c r="B40" s="120"/>
+      <c r="A40" s="119" t="s">
+        <v>276</v>
+      </c>
+      <c r="B40" s="175">
+        <f>B38*-1</f>
+        <v>46854537.664252765</v>
+      </c>
       <c r="L40" s="11"/>
       <c r="M40" s="44"/>
     </row>
     <row r="41" spans="1:13" ht="12.75">
-      <c r="B41" s="44"/>
-      <c r="L41" s="11">
+      <c r="A41" s="119" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="175">
+        <f>B32+(B39/(B39+B40))</f>
+        <v>29.213908675634876</v>
+      </c>
+      <c r="L41" s="11"/>
+      <c r="M41" s="44"/>
+    </row>
+    <row r="42" spans="1:13" ht="12.75">
+      <c r="A42" s="119"/>
+      <c r="B42" s="120"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="44"/>
+    </row>
+    <row r="43" spans="1:13" ht="12.75">
+      <c r="B43" s="44"/>
+      <c r="L43" s="11">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M41" s="44">
+      <c r="M43" s="44">
         <f t="shared" si="0"/>
         <v>855330893.90745759</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="12.75">
-      <c r="L42" s="11">
+    <row r="44" spans="1:13" ht="12.75">
+      <c r="L44" s="11">
         <v>1.1499999999999999</v>
       </c>
-      <c r="M42" s="44">
+      <c r="M44" s="44">
         <f t="shared" si="0"/>
         <v>802348473.35562515</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="12.75">
-      <c r="A43" s="119" t="s">
+    <row r="45" spans="1:13" ht="12.75">
+      <c r="A45" s="119" t="s">
         <v>265</v>
       </c>
-      <c r="B43" s="120" t="s">
+      <c r="B45" s="120" t="s">
         <v>266</v>
       </c>
-      <c r="C43" s="98" t="s">
+      <c r="C45" s="98" t="s">
         <v>267</v>
       </c>
-      <c r="L43" s="11">
+      <c r="L45" s="11">
         <v>1.2</v>
       </c>
-      <c r="M43" s="44">
+      <c r="M45" s="44">
         <f t="shared" si="0"/>
         <v>754126147.23541009</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="12.75">
-      <c r="A44" s="119" t="s">
+    <row r="46" spans="1:13" ht="12.75">
+      <c r="A46" s="119" t="s">
         <v>263</v>
       </c>
-      <c r="B44" s="120"/>
-      <c r="C44" s="98" t="s">
+      <c r="B46" s="120"/>
+      <c r="C46" s="98" t="s">
         <v>264</v>
       </c>
-      <c r="L44" s="11"/>
-    </row>
-    <row r="45" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A45" s="98" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="208">
-        <v>5.7500000000000002E-2</v>
-      </c>
-      <c r="C45" s="209">
-        <f xml:space="preserve"> 1 +B45</f>
-        <v>1.0575000000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A46" s="98" t="s">
-        <v>75</v>
-      </c>
-      <c r="B46" s="208">
-        <v>0.06</v>
-      </c>
-      <c r="C46" s="209">
-        <f t="shared" ref="C46:C49" si="1" xml:space="preserve"> 1 +B46</f>
-        <v>1.06</v>
-      </c>
+      <c r="L46" s="11"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1">
       <c r="A47" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="208">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="C47" s="209">
-        <f t="shared" si="1"/>
-        <v>1.0649999999999999</v>
+        <v>74</v>
+      </c>
+      <c r="B47" s="173">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="C47" s="174">
+        <f xml:space="preserve"> 1 +B47</f>
+        <v>1.0575000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1">
       <c r="A48" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="B48" s="208">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C48" s="209">
-        <f t="shared" si="1"/>
-        <v>1.07</v>
+        <v>75</v>
+      </c>
+      <c r="B48" s="173">
+        <v>0.06</v>
+      </c>
+      <c r="C48" s="174">
+        <f t="shared" ref="C48:C51" si="2" xml:space="preserve"> 1 +B48</f>
+        <v>1.06</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1">
       <c r="A49" s="98" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="173">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="C49" s="174">
+        <f t="shared" si="2"/>
+        <v>1.0649999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A50" s="98" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" s="173">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C50" s="174">
+        <f t="shared" si="2"/>
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A51" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="B49" s="208">
+      <c r="B51" s="173">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="C49" s="209">
-        <f t="shared" si="1"/>
+      <c r="C51" s="174">
+        <f t="shared" si="2"/>
         <v>1.0720000000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="5">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
@@ -5697,27 +5774,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A1" s="189"/>
-      <c r="B1" s="190" t="s">
+      <c r="A1" s="159"/>
+      <c r="B1" s="209" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="191"/>
-      <c r="D1" s="190" t="s">
+      <c r="C1" s="210"/>
+      <c r="D1" s="209" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="191"/>
-      <c r="F1" s="190" t="s">
+      <c r="E1" s="210"/>
+      <c r="F1" s="209" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="191"/>
-      <c r="H1" s="190" t="s">
+      <c r="G1" s="210"/>
+      <c r="H1" s="209" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="191"/>
-      <c r="J1" s="200" t="s">
+      <c r="I1" s="210"/>
+      <c r="J1" s="213" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="201"/>
+      <c r="K1" s="214"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="31" t="s">
@@ -5759,7 +5836,7 @@
         <f>K2/$K$2</f>
         <v>1</v>
       </c>
-      <c r="K2" s="202">
+      <c r="K2" s="167">
         <f>SUM(K4,K8)</f>
         <v>4032478422</v>
       </c>
@@ -5780,7 +5857,7 @@
       </c>
       <c r="I3" s="89"/>
       <c r="J3" s="90"/>
-      <c r="K3" s="203"/>
+      <c r="K3" s="168"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
       <c r="A4" s="40" t="s">
@@ -5822,7 +5899,7 @@
         <f>K4/$K$2</f>
         <v>0.9669635553972965</v>
       </c>
-      <c r="K4" s="204">
+      <c r="K4" s="169">
         <f>'Estado de resultados PyG - 5 añ'!K3</f>
         <v>3899259672</v>
       </c>
@@ -5840,7 +5917,7 @@
       <c r="H5" s="83"/>
       <c r="I5" s="89"/>
       <c r="J5" s="90"/>
-      <c r="K5" s="203"/>
+      <c r="K5" s="168"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
       <c r="A6" s="40" t="s">
@@ -5882,7 +5959,7 @@
         <f>K6/$K$2</f>
         <v>3.3904397170262154E-2</v>
       </c>
-      <c r="K6" s="204">
+      <c r="K6" s="169">
         <f>I6*2.5</f>
         <v>136718750</v>
       </c>
@@ -5927,7 +6004,7 @@
         <f>K7/$K$2</f>
         <v>8.6795256755871114E-4</v>
       </c>
-      <c r="K7" s="204">
+      <c r="K7" s="169">
         <f>I7+$C$7</f>
         <v>3500000</v>
       </c>
@@ -5949,7 +6026,7 @@
         <v>3.755135147313952E-3</v>
       </c>
       <c r="E8" s="92">
-        <f t="shared" ref="D8:K8" si="0">E6-E7</f>
+        <f t="shared" ref="E8:K8" si="0">E6-E7</f>
         <v>7350000</v>
       </c>
       <c r="F8" s="83">
@@ -5972,7 +6049,7 @@
         <f>K8/$K$2</f>
         <v>3.3036444602703441E-2</v>
       </c>
-      <c r="K8" s="204">
+      <c r="K8" s="169">
         <f t="shared" si="0"/>
         <v>133218750</v>
       </c>
@@ -6017,7 +6094,7 @@
         <f>K9/$K$9</f>
         <v>1</v>
       </c>
-      <c r="K9" s="202">
+      <c r="K9" s="167">
         <f>SUM(K11:K14)</f>
         <v>1393042105.4902561</v>
       </c>
@@ -6035,7 +6112,7 @@
       <c r="H10" s="83"/>
       <c r="I10" s="89"/>
       <c r="J10" s="90"/>
-      <c r="K10" s="203"/>
+      <c r="K10" s="168"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="40" t="s">
@@ -6077,7 +6154,7 @@
         <f>K11/$K$9</f>
         <v>5.551705845444092E-4</v>
       </c>
-      <c r="K11" s="204">
+      <c r="K11" s="169">
         <f>'Flujo de caja - 5 años'!M6</f>
         <v>773376</v>
       </c>
@@ -6122,7 +6199,7 @@
         <f>K12/$K$9</f>
         <v>0.92484663348563545</v>
       </c>
-      <c r="K12" s="204">
+      <c r="K12" s="169">
         <f>'Flujo de caja - 5 años'!M9</f>
         <v>1288350301.5664048</v>
       </c>
@@ -6167,7 +6244,7 @@
         <f>K13/$K$9</f>
         <v>7.1532260849309276E-2</v>
       </c>
-      <c r="K13" s="204">
+      <c r="K13" s="169">
         <f>'Flujo de caja - 5 años'!M3</f>
         <v>99647451.263999999</v>
       </c>
@@ -6212,7 +6289,7 @@
         <f>K14/$K$9</f>
         <v>3.0659350805108342E-3</v>
       </c>
-      <c r="K14" s="204">
+      <c r="K14" s="169">
         <f>'Flujo de caja - 5 años'!M4+'Flujo de caja - 5 años'!M5+'Flujo de caja - 5 años'!M8</f>
         <v>4270976.6598512502</v>
       </c>
@@ -6257,7 +6334,7 @@
         <f>K15/$K$15</f>
         <v>1</v>
       </c>
-      <c r="K15" s="202">
+      <c r="K15" s="167">
         <f>K16</f>
         <v>2639436316.5097437</v>
       </c>
@@ -6302,7 +6379,7 @@
         <f>K16/$K$15</f>
         <v>1</v>
       </c>
-      <c r="K16" s="205">
+      <c r="K16" s="170">
         <f>K2-K9</f>
         <v>2639436316.5097437</v>
       </c>
@@ -6394,7 +6471,7 @@
         <v>67</v>
       </c>
       <c r="B3" s="87">
-        <f>F3</f>
+        <f t="shared" ref="B3:B8" si="0">F3</f>
         <v>2671</v>
       </c>
       <c r="C3" s="118">
@@ -6425,11 +6502,11 @@
         <v>68</v>
       </c>
       <c r="B4" s="87">
-        <f>F4</f>
+        <f t="shared" si="0"/>
         <v>3380</v>
       </c>
       <c r="C4" s="118">
-        <f t="shared" ref="C4:C13" si="0">B4*(20400+(20400*0.19))</f>
+        <f t="shared" ref="C4:C13" si="1">B4*(20400+(20400*0.19))</f>
         <v>82052880</v>
       </c>
       <c r="E4">
@@ -6456,11 +6533,11 @@
         <v>69</v>
       </c>
       <c r="B5" s="87">
-        <f>F5</f>
+        <f t="shared" si="0"/>
         <v>4273</v>
       </c>
       <c r="C5" s="118">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>103731348</v>
       </c>
       <c r="E5">
@@ -6481,11 +6558,11 @@
         <v>70</v>
       </c>
       <c r="B6" s="87">
-        <f>F6</f>
+        <f t="shared" si="0"/>
         <v>5393</v>
       </c>
       <c r="C6" s="118">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>130920468</v>
       </c>
       <c r="E6">
@@ -6500,11 +6577,11 @@
         <v>71</v>
       </c>
       <c r="B7" s="87">
-        <f>F7</f>
+        <f t="shared" si="0"/>
         <v>6794</v>
       </c>
       <c r="C7" s="118">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>164931144</v>
       </c>
       <c r="E7">
@@ -6519,11 +6596,11 @@
         <v>72</v>
       </c>
       <c r="B8" s="87">
-        <f>F8</f>
+        <f t="shared" si="0"/>
         <v>8539</v>
       </c>
       <c r="C8" s="118">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>207292764</v>
       </c>
       <c r="D8" t="s">
@@ -6545,7 +6622,7 @@
         <v>8539</v>
       </c>
       <c r="C9" s="118">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>207292764</v>
       </c>
       <c r="D9" t="s">
@@ -6567,7 +6644,7 @@
         <v>80325</v>
       </c>
       <c r="C10" s="118">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1949969700</v>
       </c>
       <c r="D10" t="s">
@@ -6589,7 +6666,7 @@
         <v>152111</v>
       </c>
       <c r="C11" s="118">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3692646636</v>
       </c>
       <c r="D11" t="s">
@@ -6611,7 +6688,7 @@
         <v>160145</v>
       </c>
       <c r="C12" s="118">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3887680020</v>
       </c>
       <c r="D12" t="s">
@@ -6633,7 +6710,7 @@
         <v>160622</v>
       </c>
       <c r="C13" s="118">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3899259672</v>
       </c>
     </row>
@@ -6959,22 +7036,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A1" s="163" t="s">
+      <c r="A1" s="178" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="164"/>
-      <c r="D1" s="163" t="s">
+      <c r="B1" s="179"/>
+      <c r="D1" s="178" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="164"/>
-      <c r="G1" s="163" t="s">
+      <c r="E1" s="179"/>
+      <c r="G1" s="178" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="164"/>
-      <c r="J1" s="163" t="s">
+      <c r="H1" s="179"/>
+      <c r="J1" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="164"/>
+      <c r="K1" s="179"/>
       <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
@@ -7185,10 +7262,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A17" s="163" t="s">
+      <c r="A17" s="178" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="164"/>
+      <c r="B17" s="179"/>
       <c r="E17" s="11" t="s">
         <v>37</v>
       </c>
@@ -7349,26 +7426,26 @@
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A34" s="150" t="s">
+      <c r="A34" s="181" t="s">
         <v>220</v>
       </c>
-      <c r="B34" s="150"/>
-      <c r="C34" s="150"/>
-      <c r="D34" s="150"/>
-      <c r="E34" s="150"/>
-      <c r="F34" s="150"/>
-      <c r="G34" s="150"/>
-      <c r="H34" s="150"/>
+      <c r="B34" s="181"/>
+      <c r="C34" s="181"/>
+      <c r="D34" s="181"/>
+      <c r="E34" s="181"/>
+      <c r="F34" s="181"/>
+      <c r="G34" s="181"/>
+      <c r="H34" s="181"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A35" s="161"/>
-      <c r="B35" s="161"/>
-      <c r="C35" s="161"/>
-      <c r="D35" s="161"/>
-      <c r="E35" s="161"/>
-      <c r="F35" s="161"/>
-      <c r="G35" s="161"/>
-      <c r="H35" s="161"/>
+      <c r="A35" s="182"/>
+      <c r="B35" s="182"/>
+      <c r="C35" s="182"/>
+      <c r="D35" s="182"/>
+      <c r="E35" s="182"/>
+      <c r="F35" s="182"/>
+      <c r="G35" s="182"/>
+      <c r="H35" s="182"/>
     </row>
     <row r="36" spans="1:8" ht="46.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A36" s="113" t="s">
@@ -7574,251 +7651,256 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="46" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A46" s="150" t="s">
+      <c r="A46" s="181" t="s">
         <v>238</v>
       </c>
-      <c r="B46" s="150"/>
-      <c r="C46" s="150"/>
-      <c r="D46" s="150"/>
-      <c r="E46" s="150"/>
-      <c r="F46" s="150"/>
+      <c r="B46" s="181"/>
+      <c r="C46" s="181"/>
+      <c r="D46" s="181"/>
+      <c r="E46" s="181"/>
+      <c r="F46" s="181"/>
     </row>
     <row r="47" spans="1:8" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A47" s="162" t="s">
+      <c r="A47" s="183" t="s">
         <v>223</v>
       </c>
-      <c r="B47" s="162"/>
-      <c r="C47" s="162"/>
-      <c r="D47" s="162"/>
-      <c r="E47" s="162" t="s">
+      <c r="B47" s="183"/>
+      <c r="C47" s="183"/>
+      <c r="D47" s="183"/>
+      <c r="E47" s="183" t="s">
         <v>74</v>
       </c>
-      <c r="F47" s="162"/>
+      <c r="F47" s="183"/>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A48" s="156" t="s">
+      <c r="A48" s="185" t="s">
         <v>231</v>
       </c>
-      <c r="B48" s="158"/>
-      <c r="C48" s="153" t="s">
+      <c r="B48" s="186"/>
+      <c r="C48" s="189" t="s">
         <v>224</v>
       </c>
-      <c r="D48" s="157"/>
-      <c r="E48" s="160">
-        <v>0</v>
-      </c>
-      <c r="F48" s="160"/>
+      <c r="D48" s="190"/>
+      <c r="E48" s="180">
+        <v>0</v>
+      </c>
+      <c r="F48" s="180"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A49" s="158"/>
-      <c r="B49" s="158"/>
-      <c r="C49" s="153" t="s">
+      <c r="A49" s="186"/>
+      <c r="B49" s="186"/>
+      <c r="C49" s="189" t="s">
         <v>225</v>
       </c>
-      <c r="D49" s="157"/>
-      <c r="E49" s="160">
+      <c r="D49" s="190"/>
+      <c r="E49" s="180">
         <f>B2*12</f>
         <v>19200000</v>
       </c>
-      <c r="F49" s="160"/>
+      <c r="F49" s="180"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A50" s="158"/>
-      <c r="B50" s="158"/>
-      <c r="C50" s="153" t="s">
+      <c r="A50" s="186"/>
+      <c r="B50" s="186"/>
+      <c r="C50" s="189" t="s">
         <v>226</v>
       </c>
-      <c r="D50" s="157"/>
-      <c r="E50" s="160">
+      <c r="D50" s="190"/>
+      <c r="E50" s="180">
         <f>(B19+B22)*12</f>
         <v>39415992</v>
       </c>
-      <c r="F50" s="160"/>
+      <c r="F50" s="180"/>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A51" s="158"/>
-      <c r="B51" s="158"/>
-      <c r="C51" s="153" t="s">
+      <c r="A51" s="186"/>
+      <c r="B51" s="186"/>
+      <c r="C51" s="189" t="s">
         <v>227</v>
       </c>
-      <c r="D51" s="153"/>
-      <c r="E51" s="160">
+      <c r="D51" s="189"/>
+      <c r="E51" s="180">
         <f>B4*12</f>
         <v>2400000</v>
       </c>
-      <c r="F51" s="160"/>
+      <c r="F51" s="180"/>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A52" s="158"/>
-      <c r="B52" s="158"/>
-      <c r="C52" s="153" t="s">
+      <c r="A52" s="186"/>
+      <c r="B52" s="186"/>
+      <c r="C52" s="189" t="s">
         <v>228</v>
       </c>
-      <c r="D52" s="157"/>
-      <c r="E52" s="160">
+      <c r="D52" s="190"/>
+      <c r="E52" s="180">
         <f>(B21+B23)*12</f>
         <v>31938720</v>
       </c>
-      <c r="F52" s="160"/>
+      <c r="F52" s="180"/>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A53" s="158"/>
-      <c r="B53" s="158"/>
-      <c r="C53" s="153" t="s">
+      <c r="A53" s="186"/>
+      <c r="B53" s="186"/>
+      <c r="C53" s="189" t="s">
         <v>229</v>
       </c>
-      <c r="D53" s="157"/>
-      <c r="E53" s="160">
-        <v>0</v>
-      </c>
-      <c r="F53" s="160"/>
+      <c r="D53" s="190"/>
+      <c r="E53" s="180">
+        <v>0</v>
+      </c>
+      <c r="F53" s="180"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A54" s="158"/>
-      <c r="B54" s="158"/>
-      <c r="C54" s="150" t="s">
+      <c r="A54" s="186"/>
+      <c r="B54" s="186"/>
+      <c r="C54" s="181" t="s">
         <v>230</v>
       </c>
-      <c r="D54" s="150"/>
-      <c r="E54" s="151">
+      <c r="D54" s="181"/>
+      <c r="E54" s="184">
         <f>SUM(E48:F53)</f>
         <v>92954712</v>
       </c>
-      <c r="F54" s="151"/>
+      <c r="F54" s="184"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A55" s="156" t="s">
+      <c r="A55" s="185" t="s">
         <v>237</v>
       </c>
-      <c r="B55" s="158"/>
-      <c r="C55" s="152" t="s">
+      <c r="B55" s="186"/>
+      <c r="C55" s="187" t="s">
         <v>232</v>
       </c>
-      <c r="D55" s="159"/>
-      <c r="E55" s="154">
-        <v>0</v>
-      </c>
-      <c r="F55" s="154"/>
+      <c r="D55" s="188"/>
+      <c r="E55" s="191">
+        <v>0</v>
+      </c>
+      <c r="F55" s="191"/>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A56" s="158"/>
-      <c r="B56" s="158"/>
-      <c r="C56" s="153" t="s">
+      <c r="A56" s="186"/>
+      <c r="B56" s="186"/>
+      <c r="C56" s="189" t="s">
         <v>233</v>
       </c>
-      <c r="D56" s="157"/>
-      <c r="E56" s="155">
+      <c r="D56" s="190"/>
+      <c r="E56" s="192">
         <f>'Presupuesto Inicial'!J20*12</f>
         <v>700000</v>
       </c>
-      <c r="F56" s="155"/>
+      <c r="F56" s="192"/>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A57" s="158"/>
-      <c r="B57" s="158"/>
-      <c r="C57" s="153" t="s">
+      <c r="A57" s="186"/>
+      <c r="B57" s="186"/>
+      <c r="C57" s="189" t="s">
         <v>234</v>
       </c>
-      <c r="D57" s="157"/>
-      <c r="E57" s="155">
-        <v>0</v>
-      </c>
-      <c r="F57" s="155"/>
+      <c r="D57" s="190"/>
+      <c r="E57" s="192">
+        <v>0</v>
+      </c>
+      <c r="F57" s="192"/>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A58" s="158"/>
-      <c r="B58" s="158"/>
-      <c r="C58" s="153" t="s">
+      <c r="A58" s="186"/>
+      <c r="B58" s="186"/>
+      <c r="C58" s="189" t="s">
         <v>235</v>
       </c>
-      <c r="D58" s="157"/>
-      <c r="E58" s="155">
-        <v>0</v>
-      </c>
-      <c r="F58" s="155"/>
+      <c r="D58" s="190"/>
+      <c r="E58" s="192">
+        <v>0</v>
+      </c>
+      <c r="F58" s="192"/>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A59" s="158"/>
-      <c r="B59" s="158"/>
-      <c r="C59" s="150" t="s">
+      <c r="A59" s="186"/>
+      <c r="B59" s="186"/>
+      <c r="C59" s="181" t="s">
         <v>236</v>
       </c>
-      <c r="D59" s="150"/>
-      <c r="E59" s="151">
+      <c r="D59" s="181"/>
+      <c r="E59" s="184">
         <f>SUM(E55:F58)</f>
         <v>700000</v>
       </c>
-      <c r="F59" s="150"/>
+      <c r="F59" s="181"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A60" s="156" t="s">
+      <c r="A60" s="185" t="s">
         <v>241</v>
       </c>
-      <c r="B60" s="156"/>
-      <c r="C60" s="152" t="s">
+      <c r="B60" s="185"/>
+      <c r="C60" s="187" t="s">
         <v>251</v>
       </c>
-      <c r="D60" s="152"/>
-      <c r="E60" s="154">
+      <c r="D60" s="187"/>
+      <c r="E60" s="191">
         <f>('Presupuesto Inicial'!B12+'Presupuesto Inicial'!B13)+('Presupuesto Inicial'!B11*6)+('Salarios, gastos y costos'!K11*12)</f>
         <v>7848920</v>
       </c>
-      <c r="F60" s="154"/>
+      <c r="F60" s="191"/>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A61" s="156"/>
-      <c r="B61" s="156"/>
-      <c r="C61" s="153" t="s">
+      <c r="A61" s="185"/>
+      <c r="B61" s="185"/>
+      <c r="C61" s="189" t="s">
         <v>239</v>
       </c>
-      <c r="D61" s="153"/>
-      <c r="E61" s="155">
+      <c r="D61" s="189"/>
+      <c r="E61" s="192">
         <f>'Presupuesto Inicial'!B2</f>
         <v>116700</v>
       </c>
-      <c r="F61" s="155"/>
+      <c r="F61" s="192"/>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A62" s="156"/>
-      <c r="B62" s="156"/>
-      <c r="C62" s="150" t="s">
+      <c r="A62" s="185"/>
+      <c r="B62" s="185"/>
+      <c r="C62" s="181" t="s">
         <v>240</v>
       </c>
-      <c r="D62" s="150"/>
-      <c r="E62" s="151">
+      <c r="D62" s="181"/>
+      <c r="E62" s="184">
         <f>E60+E61</f>
         <v>7965620</v>
       </c>
-      <c r="F62" s="151"/>
+      <c r="F62" s="184"/>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A63" s="150" t="s">
+      <c r="A63" s="181" t="s">
         <v>245</v>
       </c>
-      <c r="B63" s="150"/>
-      <c r="C63" s="150"/>
-      <c r="D63" s="150"/>
-      <c r="E63" s="151">
+      <c r="B63" s="181"/>
+      <c r="C63" s="181"/>
+      <c r="D63" s="181"/>
+      <c r="E63" s="184">
         <f>E54+E59+E62</f>
         <v>101620332</v>
       </c>
-      <c r="F63" s="151"/>
+      <c r="F63" s="184"/>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" thickTop="1"/>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A35:H35"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="A60:B62"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
     <mergeCell ref="C54:D54"/>
     <mergeCell ref="E54:F54"/>
     <mergeCell ref="A48:B54"/>
@@ -7835,23 +7917,18 @@
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="E50:F50"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="A60:B62"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A35:H35"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F31" r:id="rId1"/>
@@ -7881,28 +7958,28 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="181" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="165"/>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
+      <c r="B2" s="193"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" thickTop="1">
-      <c r="A3" s="167" t="s">
+      <c r="A3" s="195" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="164"/>
-      <c r="C3" s="167" t="s">
+      <c r="B3" s="179"/>
+      <c r="C3" s="195" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="164"/>
+      <c r="D3" s="179"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A4" s="168" t="s">
+      <c r="A4" s="196" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="171">
+      <c r="B4" s="199">
         <v>1500000</v>
       </c>
       <c r="C4" s="19" t="s">
@@ -7913,16 +7990,16 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A5" s="169"/>
-      <c r="B5" s="169"/>
-      <c r="C5" s="167" t="s">
+      <c r="A5" s="197"/>
+      <c r="B5" s="197"/>
+      <c r="C5" s="195" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="164"/>
+      <c r="D5" s="179"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A6" s="169"/>
-      <c r="B6" s="169"/>
+      <c r="A6" s="197"/>
+      <c r="B6" s="197"/>
       <c r="C6" s="19" t="s">
         <v>40</v>
       </c>
@@ -7931,8 +8008,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A7" s="169"/>
-      <c r="B7" s="169"/>
+      <c r="A7" s="197"/>
+      <c r="B7" s="197"/>
       <c r="C7" s="19" t="s">
         <v>43</v>
       </c>
@@ -7941,8 +8018,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1">
-      <c r="A8" s="170"/>
-      <c r="B8" s="170"/>
+      <c r="A8" s="198"/>
+      <c r="B8" s="198"/>
       <c r="C8" s="19" t="s">
         <v>242</v>
       </c>
@@ -7967,15 +8044,15 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A10" s="150" t="s">
+      <c r="A10" s="181" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="165"/>
-      <c r="C10" s="166">
+      <c r="B10" s="193"/>
+      <c r="C10" s="194">
         <f>D4+D9</f>
         <v>1500000</v>
       </c>
-      <c r="D10" s="165"/>
+      <c r="D10" s="193"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" thickTop="1"/>
     <row r="12" spans="1:4" ht="15.75" customHeight="1">
@@ -8011,49 +8088,49 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="15">
-      <c r="B2" s="172" t="s">
+      <c r="B2" s="200" t="s">
         <v>244</v>
       </c>
-      <c r="C2" s="172"/>
-      <c r="D2" s="172"/>
-      <c r="E2" s="172"/>
-      <c r="F2" s="172"/>
+      <c r="C2" s="200"/>
+      <c r="D2" s="200"/>
+      <c r="E2" s="200"/>
+      <c r="F2" s="200"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="161" t="s">
+      <c r="B3" s="182" t="s">
         <v>246</v>
       </c>
-      <c r="C3" s="161"/>
-      <c r="D3" s="161"/>
-      <c r="E3" s="174">
+      <c r="C3" s="182"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="202">
         <f>'Salarios, gastos y costos'!E62:F62</f>
         <v>7965620</v>
       </c>
-      <c r="F3" s="174"/>
+      <c r="F3" s="202"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="175" t="s">
+      <c r="B4" s="203" t="s">
         <v>247</v>
       </c>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="176">
+      <c r="C4" s="182"/>
+      <c r="D4" s="182"/>
+      <c r="E4" s="204">
         <f>'Salarios, gastos y costos'!B11*7</f>
         <v>54223582</v>
       </c>
-      <c r="F4" s="176"/>
+      <c r="F4" s="204"/>
     </row>
     <row r="5" spans="2:6" ht="15">
-      <c r="B5" s="172" t="s">
+      <c r="B5" s="200" t="s">
         <v>214</v>
       </c>
-      <c r="C5" s="172"/>
-      <c r="D5" s="172"/>
-      <c r="E5" s="173">
+      <c r="C5" s="200"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="201">
         <f>SUM(E3:F4)</f>
         <v>62189202</v>
       </c>
-      <c r="F5" s="173"/>
+      <c r="F5" s="201"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -8124,30 +8201,30 @@
       <c r="G1" s="130" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="178" t="s">
+      <c r="H1" s="206" t="s">
         <v>67</v>
       </c>
-      <c r="I1" s="164"/>
-      <c r="J1" s="177" t="s">
+      <c r="I1" s="179"/>
+      <c r="J1" s="205" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="164"/>
-      <c r="L1" s="177" t="s">
+      <c r="K1" s="179"/>
+      <c r="L1" s="205" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="164"/>
-      <c r="N1" s="177" t="s">
+      <c r="M1" s="179"/>
+      <c r="N1" s="205" t="s">
         <v>70</v>
       </c>
-      <c r="O1" s="164"/>
-      <c r="P1" s="177" t="s">
+      <c r="O1" s="179"/>
+      <c r="P1" s="205" t="s">
         <v>71</v>
       </c>
-      <c r="Q1" s="164"/>
-      <c r="R1" s="177" t="s">
+      <c r="Q1" s="179"/>
+      <c r="R1" s="205" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="164"/>
+      <c r="S1" s="179"/>
       <c r="U1" s="147" t="s">
         <v>74</v>
       </c>
@@ -8961,7 +9038,7 @@
         <f t="shared" si="1"/>
         <v>651116373.51127625</v>
       </c>
-      <c r="V11" s="192">
+      <c r="V11" s="160">
         <f>S11+Q11+O11+M11+K11+I11</f>
         <v>701195583.99999988</v>
       </c>
@@ -9034,7 +9111,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V12" s="192">
+      <c r="V12" s="160">
         <f t="shared" ref="V12:V14" si="11">S12+Q12+O12+M12+K12+I12</f>
         <v>0</v>
       </c>
@@ -9107,7 +9184,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V13" s="192">
+      <c r="V13" s="160">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -9192,7 +9269,7 @@
         <f t="shared" si="1"/>
         <v>651116373.51127625</v>
       </c>
-      <c r="V14" s="192">
+      <c r="V14" s="160">
         <f t="shared" si="11"/>
         <v>701195583.99999988</v>
       </c>
@@ -9277,7 +9354,7 @@
         <f t="shared" si="1"/>
         <v>238406500.43383396</v>
       </c>
-      <c r="V15" s="193">
+      <c r="V15" s="161">
         <f>V14*0.34</f>
         <v>238406498.55999997</v>
       </c>
@@ -9491,7 +9568,7 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:K21"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -9508,26 +9585,26 @@
   <sheetData>
     <row r="1" spans="1:18" ht="12.75">
       <c r="A1" s="26"/>
-      <c r="B1" s="177" t="s">
+      <c r="B1" s="205" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="164"/>
-      <c r="D1" s="177" t="s">
+      <c r="C1" s="179"/>
+      <c r="D1" s="205" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="164"/>
-      <c r="F1" s="177" t="s">
+      <c r="E1" s="179"/>
+      <c r="F1" s="205" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="164"/>
-      <c r="H1" s="177" t="s">
+      <c r="G1" s="179"/>
+      <c r="H1" s="205" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="164"/>
-      <c r="J1" s="179" t="s">
+      <c r="I1" s="179"/>
+      <c r="J1" s="207" t="s">
         <v>79</v>
       </c>
-      <c r="K1" s="180"/>
+      <c r="K1" s="208"/>
       <c r="L1" s="28"/>
       <c r="M1" s="28"/>
       <c r="N1" s="28"/>
@@ -10458,60 +10535,60 @@
     <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="186" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A1" s="189"/>
-      <c r="B1" s="190" t="s">
+    <row r="1" spans="1:29" s="156" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A1" s="159"/>
+      <c r="B1" s="209" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="191"/>
-      <c r="D1" s="190" t="s">
+      <c r="C1" s="210"/>
+      <c r="D1" s="209" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="191"/>
-      <c r="F1" s="190" t="s">
+      <c r="E1" s="210"/>
+      <c r="F1" s="209" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="191"/>
-      <c r="H1" s="190" t="s">
+      <c r="G1" s="210"/>
+      <c r="H1" s="209" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="191"/>
-      <c r="J1" s="190" t="s">
+      <c r="I1" s="210"/>
+      <c r="J1" s="209" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="191"/>
-      <c r="L1" s="190" t="s">
+      <c r="K1" s="210"/>
+      <c r="L1" s="209" t="s">
         <v>65</v>
       </c>
-      <c r="M1" s="191"/>
-      <c r="N1" s="190" t="s">
+      <c r="M1" s="210"/>
+      <c r="N1" s="209" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="191"/>
-      <c r="P1" s="190" t="s">
+      <c r="O1" s="210"/>
+      <c r="P1" s="209" t="s">
         <v>67</v>
       </c>
-      <c r="Q1" s="191"/>
-      <c r="R1" s="190" t="s">
+      <c r="Q1" s="210"/>
+      <c r="R1" s="209" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="191"/>
-      <c r="T1" s="190" t="s">
+      <c r="S1" s="210"/>
+      <c r="T1" s="209" t="s">
         <v>69</v>
       </c>
-      <c r="U1" s="191"/>
-      <c r="V1" s="190" t="s">
+      <c r="U1" s="210"/>
+      <c r="V1" s="209" t="s">
         <v>70</v>
       </c>
-      <c r="W1" s="191"/>
-      <c r="X1" s="190" t="s">
+      <c r="W1" s="210"/>
+      <c r="X1" s="209" t="s">
         <v>71</v>
       </c>
-      <c r="Y1" s="191"/>
-      <c r="Z1" s="190" t="s">
+      <c r="Y1" s="210"/>
+      <c r="Z1" s="209" t="s">
         <v>72</v>
       </c>
-      <c r="AA1" s="191"/>
+      <c r="AA1" s="210"/>
     </row>
     <row r="2" spans="1:29" ht="15.75" customHeight="1">
       <c r="A2" s="31" t="s">
@@ -10537,7 +10614,7 @@
         <f t="shared" ref="F2:F9" si="2">G2/$G$2</f>
         <v>1</v>
       </c>
-      <c r="G2" s="183">
+      <c r="G2" s="153">
         <f>SUM(G3:G9)</f>
         <v>8249036</v>
       </c>
@@ -10545,7 +10622,7 @@
         <f t="shared" ref="H2:H9" si="3">I2/$I$2</f>
         <v>1</v>
       </c>
-      <c r="I2" s="183">
+      <c r="I2" s="153">
         <f>SUM(I3:I9)</f>
         <v>8279036</v>
       </c>
@@ -10553,7 +10630,7 @@
         <f t="shared" ref="J2:J9" si="4">K2/$K$2</f>
         <v>1</v>
       </c>
-      <c r="K2" s="183">
+      <c r="K2" s="153">
         <f>SUM(K3:K9)</f>
         <v>8179036</v>
       </c>
@@ -10621,7 +10698,7 @@
         <f>SUM(AA3:AA9)</f>
         <v>76204370.186666667</v>
       </c>
-      <c r="AC2" s="182">
+      <c r="AC2" s="152">
         <f t="shared" ref="AC2:AC6" si="13">AA2+Y2+W2+U2+S2+Q2+O2+M2+K2+I2+G2+E2</f>
         <v>340359930.56</v>
       </c>
@@ -10649,7 +10726,7 @@
         <f t="shared" si="2"/>
         <v>0.93904621097544005</v>
       </c>
-      <c r="G3" s="184">
+      <c r="G3" s="154">
         <f>'Salarios, gastos y costos'!$B$11</f>
         <v>7746226</v>
       </c>
@@ -10657,7 +10734,7 @@
         <f t="shared" si="3"/>
         <v>0.93564347346720078</v>
       </c>
-      <c r="I3" s="184">
+      <c r="I3" s="154">
         <f>'Salarios, gastos y costos'!$B$11</f>
         <v>7746226</v>
       </c>
@@ -10665,7 +10742,7 @@
         <f t="shared" si="4"/>
         <v>0.94708300587012939</v>
       </c>
-      <c r="K3" s="184">
+      <c r="K3" s="154">
         <f>'Salarios, gastos y costos'!$B$11</f>
         <v>7746226</v>
       </c>
@@ -10733,7 +10810,7 @@
         <f>'Salarios, gastos y costos'!$B$27</f>
         <v>7746226</v>
       </c>
-      <c r="AC3" s="182">
+      <c r="AC3" s="152">
         <f t="shared" si="13"/>
         <v>92954712</v>
       </c>
@@ -10761,7 +10838,7 @@
         <f t="shared" si="2"/>
         <v>4.02483393211037E-2</v>
       </c>
-      <c r="G4" s="184">
+      <c r="G4" s="154">
         <f>'Salarios, gastos y costos'!$K$11</f>
         <v>332010</v>
       </c>
@@ -10769,7 +10846,7 @@
         <f t="shared" si="3"/>
         <v>4.010249502478308E-2</v>
       </c>
-      <c r="I4" s="184">
+      <c r="I4" s="154">
         <f>'Salarios, gastos y costos'!$K$11</f>
         <v>332010</v>
       </c>
@@ -10777,7 +10854,7 @@
         <f t="shared" si="4"/>
         <v>4.0592803357266061E-2</v>
       </c>
-      <c r="K4" s="184">
+      <c r="K4" s="154">
         <f>'Salarios, gastos y costos'!$K$11</f>
         <v>332010</v>
       </c>
@@ -10845,7 +10922,7 @@
         <f>'Salarios, gastos y costos'!$K$11</f>
         <v>332010</v>
       </c>
-      <c r="AC4" s="182">
+      <c r="AC4" s="152">
         <f t="shared" si="13"/>
         <v>3984120</v>
       </c>
@@ -10874,7 +10951,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G5" s="184">
+      <c r="G5" s="154">
         <f>'Salarios, gastos y costos'!$E$11</f>
         <v>0</v>
       </c>
@@ -10882,7 +10959,7 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I5" s="184">
+      <c r="I5" s="154">
         <f>'Salarios, gastos y costos'!$E$11</f>
         <v>0</v>
       </c>
@@ -10890,7 +10967,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K5" s="184">
+      <c r="K5" s="154">
         <f>'Salarios, gastos y costos'!$E$11</f>
         <v>0</v>
       </c>
@@ -10958,7 +11035,7 @@
         <f>'Salarios, gastos y costos'!$E$11</f>
         <v>0</v>
       </c>
-      <c r="AC5" s="182">
+      <c r="AC5" s="152">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
@@ -10987,7 +11064,7 @@
         <f t="shared" si="2"/>
         <v>7.3705582082560922E-3</v>
       </c>
-      <c r="G6" s="184">
+      <c r="G6" s="154">
         <f>'Salarios, gastos y costos'!$H$11</f>
         <v>60800</v>
       </c>
@@ -10995,7 +11072,7 @@
         <f t="shared" si="3"/>
         <v>7.3438501777260056E-3</v>
       </c>
-      <c r="I6" s="184">
+      <c r="I6" s="154">
         <f>'Salarios, gastos y costos'!$H$11</f>
         <v>60800</v>
       </c>
@@ -11003,7 +11080,7 @@
         <f t="shared" si="4"/>
         <v>7.4336388787138242E-3</v>
       </c>
-      <c r="K6" s="184">
+      <c r="K6" s="154">
         <f>'Salarios, gastos y costos'!$H$11</f>
         <v>60800</v>
       </c>
@@ -11071,7 +11148,7 @@
         <f>'Salarios, gastos y costos'!$H$11</f>
         <v>60800</v>
       </c>
-      <c r="AC6" s="182">
+      <c r="AC6" s="152">
         <f t="shared" si="13"/>
         <v>729600</v>
       </c>
@@ -11098,7 +11175,7 @@
         <f>G7/$C$2</f>
         <v>2.9911624745071381E-2</v>
       </c>
-      <c r="G7" s="184">
+      <c r="G7" s="154">
         <f>'Salarios, gastos y costos'!G37</f>
         <v>110000</v>
       </c>
@@ -11106,7 +11183,7 @@
         <f>I7/$C$2</f>
         <v>3.8069340584636305E-2</v>
       </c>
-      <c r="I7" s="184">
+      <c r="I7" s="154">
         <f>'Salarios, gastos y costos'!G38</f>
         <v>140000</v>
       </c>
@@ -11114,7 +11191,7 @@
         <f>K7/$C$2</f>
         <v>1.0876954452753228E-2</v>
       </c>
-      <c r="K7" s="184">
+      <c r="K7" s="154">
         <f>'Salarios, gastos y costos'!G39</f>
         <v>40000</v>
       </c>
@@ -11182,7 +11259,7 @@
         <f>'Salarios, gastos y costos'!$F$41+'Salarios, gastos y costos'!$F$42</f>
         <v>565000</v>
       </c>
-      <c r="AC7" s="182">
+      <c r="AC7" s="152">
         <f>AA7+Y7+W7+U7+S7+Q7+O7+M7+K7+I7+G7+E7</f>
         <v>4285000</v>
       </c>
@@ -11210,21 +11287,21 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G8" s="185">
+      <c r="G8" s="155">
         <v>0</v>
       </c>
       <c r="H8" s="64">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I8" s="185">
+      <c r="I8" s="155">
         <v>0</v>
       </c>
       <c r="J8" s="64">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K8" s="185">
+      <c r="K8" s="155">
         <v>0</v>
       </c>
       <c r="L8" s="41">
@@ -11283,7 +11360,7 @@
       <c r="AA8" s="54">
         <v>0</v>
       </c>
-      <c r="AC8" s="182">
+      <c r="AC8" s="152">
         <f t="shared" ref="AC8:AC13" si="14">AA8+Y8+W8+U8+S8+Q8+O8+M8+K8+I8+G8+E8</f>
         <v>0</v>
       </c>
@@ -11310,21 +11387,21 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G9" s="185">
+      <c r="G9" s="155">
         <v>0</v>
       </c>
       <c r="H9" s="64">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I9" s="185">
+      <c r="I9" s="155">
         <v>0</v>
       </c>
       <c r="J9" s="64">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K9" s="185">
+      <c r="K9" s="155">
         <v>0</v>
       </c>
       <c r="L9" s="41">
@@ -11389,7 +11466,7 @@
         <f>'Estado de resultados PyG - 12 m'!S15</f>
         <v>67500334.186666667</v>
       </c>
-      <c r="AC9" s="182">
+      <c r="AC9" s="152">
         <f t="shared" si="14"/>
         <v>238406498.56</v>
       </c>
@@ -11416,21 +11493,21 @@
       <c r="F10" s="63">
         <v>0</v>
       </c>
-      <c r="G10" s="183">
+      <c r="G10" s="153">
         <f>SUM(G11:G12)</f>
         <v>0</v>
       </c>
       <c r="H10" s="63">
         <v>0</v>
       </c>
-      <c r="I10" s="183">
+      <c r="I10" s="153">
         <f>SUM(I11:I12)</f>
         <v>0</v>
       </c>
       <c r="J10" s="63">
         <v>0</v>
       </c>
-      <c r="K10" s="183">
+      <c r="K10" s="153">
         <f>SUM(K11:K12)</f>
         <v>0</v>
       </c>
@@ -11496,7 +11573,7 @@
         <f>SUM(AA11:AA12)</f>
         <v>207292764</v>
       </c>
-      <c r="AC10" s="182">
+      <c r="AC10" s="152">
         <f t="shared" si="14"/>
         <v>753769800</v>
       </c>
@@ -11521,19 +11598,19 @@
       <c r="F11" s="64">
         <v>0</v>
       </c>
-      <c r="G11" s="185">
+      <c r="G11" s="155">
         <v>0</v>
       </c>
       <c r="H11" s="64">
         <v>0</v>
       </c>
-      <c r="I11" s="185">
+      <c r="I11" s="155">
         <v>0</v>
       </c>
       <c r="J11" s="64">
         <v>0</v>
       </c>
-      <c r="K11" s="185">
+      <c r="K11" s="155">
         <v>0</v>
       </c>
       <c r="L11" s="41">
@@ -11596,7 +11673,7 @@
         <f>'Estado de resultados PyG - 12 m'!S3</f>
         <v>207292764</v>
       </c>
-      <c r="AC11" s="182">
+      <c r="AC11" s="152">
         <f t="shared" si="14"/>
         <v>753769800</v>
       </c>
@@ -11621,19 +11698,19 @@
       <c r="F12" s="64">
         <v>0</v>
       </c>
-      <c r="G12" s="185">
+      <c r="G12" s="155">
         <v>0</v>
       </c>
       <c r="H12" s="64">
         <v>0</v>
       </c>
-      <c r="I12" s="185">
+      <c r="I12" s="155">
         <v>0</v>
       </c>
       <c r="J12" s="64">
         <v>0</v>
       </c>
-      <c r="K12" s="185">
+      <c r="K12" s="155">
         <v>0</v>
       </c>
       <c r="L12" s="41">
@@ -11684,81 +11761,81 @@
       <c r="AA12" s="54">
         <v>0</v>
       </c>
-      <c r="AC12" s="182">
+      <c r="AC12" s="152">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:29" s="186" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A13" s="186" t="s">
+    <row r="13" spans="1:29" s="156" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A13" s="156" t="s">
         <v>98</v>
       </c>
-      <c r="B13" s="187"/>
-      <c r="C13" s="187">
+      <c r="B13" s="157"/>
+      <c r="C13" s="157">
         <f>C10-C2</f>
         <v>58512500</v>
       </c>
-      <c r="D13" s="187"/>
-      <c r="E13" s="187">
+      <c r="D13" s="157"/>
+      <c r="E13" s="157">
         <f>C13-E2+E10</f>
         <v>50373464</v>
       </c>
-      <c r="F13" s="187"/>
-      <c r="G13" s="188">
+      <c r="F13" s="157"/>
+      <c r="G13" s="158">
         <f>E13-G2+G10</f>
         <v>42124428</v>
       </c>
-      <c r="H13" s="187"/>
-      <c r="I13" s="188">
+      <c r="H13" s="157"/>
+      <c r="I13" s="158">
         <f>G13-I2+I10</f>
         <v>33845392</v>
       </c>
-      <c r="J13" s="187"/>
-      <c r="K13" s="188">
+      <c r="J13" s="157"/>
+      <c r="K13" s="158">
         <f>I13-K2+K10</f>
         <v>25666356</v>
       </c>
-      <c r="L13" s="187"/>
-      <c r="M13" s="187">
+      <c r="L13" s="157"/>
+      <c r="M13" s="157">
         <f>K13-M2+M10</f>
         <v>17487320</v>
       </c>
-      <c r="N13" s="187"/>
-      <c r="O13" s="187">
+      <c r="N13" s="157"/>
+      <c r="O13" s="157">
         <f>M13-O2+O10</f>
         <v>8783284</v>
       </c>
-      <c r="P13" s="187"/>
-      <c r="Q13" s="187">
+      <c r="P13" s="157"/>
+      <c r="Q13" s="157">
         <f>O13-Q2+Q10</f>
         <v>45853642.933333337</v>
       </c>
-      <c r="R13" s="187"/>
-      <c r="S13" s="187">
+      <c r="R13" s="157"/>
+      <c r="S13" s="157">
         <f>Q13-S2+S10</f>
         <v>94283713.306666672</v>
       </c>
-      <c r="T13" s="187"/>
-      <c r="U13" s="187">
+      <c r="T13" s="157"/>
+      <c r="U13" s="157">
         <f>S13-U2+U10</f>
         <v>157021572.56</v>
       </c>
-      <c r="V13" s="187"/>
-      <c r="W13" s="187">
+      <c r="V13" s="157"/>
+      <c r="W13" s="157">
         <f>U13-W2+W10</f>
         <v>237704251.01333332</v>
       </c>
-      <c r="X13" s="187"/>
-      <c r="Y13" s="187">
+      <c r="X13" s="157"/>
+      <c r="Y13" s="157">
         <f>W13-Y2+Y10</f>
         <v>340833975.62666667</v>
       </c>
-      <c r="Z13" s="187"/>
-      <c r="AA13" s="187">
+      <c r="Z13" s="157"/>
+      <c r="AA13" s="157">
         <f>Y13-AA2+AA10</f>
         <v>471922369.44</v>
       </c>
-      <c r="AC13" s="188">
+      <c r="AC13" s="158">
         <f t="shared" si="14"/>
         <v>1525899768.8799999</v>
       </c>
@@ -11770,6 +11847,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="T1:U1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="H1:I1"/>
@@ -11777,12 +11860,6 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="T1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11811,30 +11888,30 @@
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" customHeight="1">
       <c r="A1" s="27"/>
-      <c r="B1" s="181" t="s">
+      <c r="B1" s="211" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="164"/>
-      <c r="D1" s="181" t="s">
+      <c r="C1" s="179"/>
+      <c r="D1" s="211" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="164"/>
-      <c r="F1" s="181" t="s">
+      <c r="E1" s="179"/>
+      <c r="F1" s="211" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="164"/>
-      <c r="H1" s="181" t="s">
+      <c r="G1" s="179"/>
+      <c r="H1" s="211" t="s">
         <v>76</v>
       </c>
-      <c r="I1" s="164"/>
-      <c r="J1" s="181" t="s">
+      <c r="I1" s="179"/>
+      <c r="J1" s="211" t="s">
         <v>78</v>
       </c>
-      <c r="K1" s="164"/>
-      <c r="L1" s="181" t="s">
+      <c r="K1" s="179"/>
+      <c r="L1" s="211" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="164"/>
+      <c r="M1" s="179"/>
       <c r="N1" s="29"/>
       <c r="O1" s="29"/>
       <c r="P1" s="29"/>
@@ -12541,8 +12618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -12559,26 +12636,26 @@
     <row r="1" spans="1:19" ht="12.75">
       <c r="A1" s="26"/>
       <c r="B1" s="26"/>
-      <c r="C1" s="177" t="s">
+      <c r="C1" s="205" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="164"/>
-      <c r="E1" s="177" t="s">
+      <c r="D1" s="179"/>
+      <c r="E1" s="205" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="164"/>
-      <c r="G1" s="177" t="s">
+      <c r="F1" s="179"/>
+      <c r="G1" s="205" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="164"/>
-      <c r="I1" s="177" t="s">
+      <c r="H1" s="179"/>
+      <c r="I1" s="205" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="164"/>
-      <c r="K1" s="179" t="s">
+      <c r="J1" s="179"/>
+      <c r="K1" s="207" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="194"/>
+      <c r="L1" s="212"/>
       <c r="M1" s="28"/>
       <c r="N1" s="28"/>
       <c r="O1" s="28"/>
@@ -12623,7 +12700,7 @@
       <c r="K2" s="36">
         <v>1</v>
       </c>
-      <c r="L2" s="195">
+      <c r="L2" s="162">
         <f>L3</f>
         <v>3899259672</v>
       </c>
@@ -12665,13 +12742,13 @@
         <v>1</v>
       </c>
       <c r="J3" s="49">
-        <f t="shared" ref="I3:L3" si="0">J22*$F$23</f>
+        <f t="shared" ref="J3:L3" si="0">J22*$F$23</f>
         <v>3887680020</v>
       </c>
       <c r="K3" s="51">
         <v>1</v>
       </c>
-      <c r="L3" s="196">
+      <c r="L3" s="163">
         <f t="shared" si="0"/>
         <v>3899259672</v>
       </c>
@@ -12724,7 +12801,7 @@
         <f t="shared" ref="K4:K19" si="4">(L4)/$L$2</f>
         <v>2.5935585462593422E-2</v>
       </c>
-      <c r="L4" s="195">
+      <c r="L4" s="162">
         <f>SUM(L5:L7)</f>
         <v>101129582.464</v>
       </c>
@@ -12830,7 +12907,7 @@
         <f t="shared" si="4"/>
         <v>2.5555479666961766E-2</v>
       </c>
-      <c r="L6" s="196">
+      <c r="L6" s="163">
         <f>('Salarios, gastos y costos'!$B$27)*12+(('Salarios, gastos y costos'!B11*12)*L25)</f>
         <v>99647451.263999999</v>
       </c>
@@ -12883,7 +12960,7 @@
         <f t="shared" si="4"/>
         <v>1.7952125759322857E-4</v>
       </c>
-      <c r="L7" s="196">
+      <c r="L7" s="163">
         <f>('Presupuesto Inicial'!$J$20)*12</f>
         <v>700000</v>
       </c>
@@ -12936,7 +13013,7 @@
         <f t="shared" si="4"/>
         <v>0.97406441453740655</v>
       </c>
-      <c r="L8" s="195">
+      <c r="L8" s="162">
         <f>L2-L4</f>
         <v>3798130089.5359998</v>
       </c>
@@ -12989,7 +13066,7 @@
         <f t="shared" si="4"/>
         <v>1.0953301444683191E-3</v>
       </c>
-      <c r="L9" s="196">
+      <c r="L9" s="163">
         <f>'Estado de resultados PyG - 12 m'!U9+('Estado de resultados PyG - 12 m'!U9*L25)</f>
         <v>4270976.6598512502</v>
       </c>
@@ -13042,7 +13119,7 @@
         <f t="shared" si="4"/>
         <v>1.178049276063188E-3</v>
       </c>
-      <c r="L10" s="196">
+      <c r="L10" s="163">
         <f>('Estado de resultados PyG - 12 m'!$U$10)+('Estado de resultados PyG - 12 m'!$U$10*L25)</f>
         <v>4593520.0337819839</v>
       </c>
@@ -13095,7 +13172,7 @@
         <f t="shared" si="4"/>
         <v>0.97179103511687503</v>
       </c>
-      <c r="L11" s="195">
+      <c r="L11" s="162">
         <f>L8-L9-L10</f>
         <v>3789265592.8423667</v>
       </c>
@@ -13144,7 +13221,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L12" s="196">
+      <c r="L12" s="163">
         <v>0</v>
       </c>
       <c r="M12" s="53"/>
@@ -13193,7 +13270,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L13" s="196">
+      <c r="L13" s="163">
         <v>0</v>
       </c>
       <c r="M13" s="53"/>
@@ -13245,7 +13322,7 @@
         <f t="shared" si="4"/>
         <v>0.97179103511687503</v>
       </c>
-      <c r="L14" s="195">
+      <c r="L14" s="162">
         <f>L11+L12-L13</f>
         <v>3789265592.8423667</v>
       </c>
@@ -13298,7 +13375,7 @@
         <f t="shared" si="4"/>
         <v>0.33040895193973757</v>
       </c>
-      <c r="L15" s="196">
+      <c r="L15" s="163">
         <f>IF(L14&gt;0, L14*0.34, 0)</f>
         <v>1288350301.5664048</v>
       </c>
@@ -13351,7 +13428,7 @@
         <f t="shared" si="4"/>
         <v>0.64138208317713752</v>
       </c>
-      <c r="L16" s="195">
+      <c r="L16" s="162">
         <f>L14-L15</f>
         <v>2500915291.2759619</v>
       </c>
@@ -13406,7 +13483,7 @@
         <f t="shared" si="4"/>
         <v>1.7952125759322857E-4</v>
       </c>
-      <c r="L17" s="197">
+      <c r="L17" s="164">
         <f>L7</f>
         <v>700000</v>
       </c>
@@ -13450,7 +13527,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="L18" s="198">
+      <c r="L18" s="165">
         <v>0</v>
       </c>
     </row>
@@ -13498,7 +13575,7 @@
         <f t="shared" si="4"/>
         <v>0.64156160443473076</v>
       </c>
-      <c r="L19" s="199">
+      <c r="L19" s="166">
         <f>L18+L17+L16</f>
         <v>2501615291.2759619</v>
       </c>

</xml_diff>